<commit_message>
el numero de página ya funciona
</commit_message>
<xml_diff>
--- a/RegistroVisitantes/RegistroVisitantes/Reporte.xlsx
+++ b/RegistroVisitantes/RegistroVisitantes/Reporte.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Compañía</t>
   </si>
@@ -50,6 +50,15 @@
     <t>CRO141</t>
   </si>
   <si>
+    <t>COSTA RICAN</t>
+  </si>
+  <si>
+    <t>Jeffry Venegas</t>
+  </si>
+  <si>
+    <t>jeffvene@gmail.com</t>
+  </si>
+  <si>
     <t>BELGIAN</t>
   </si>
   <si>
@@ -59,13 +68,118 @@
     <t>ddierick@fiu.edu</t>
   </si>
   <si>
-    <t>COSTA RICAN</t>
-  </si>
-  <si>
-    <t>Jeffry Venegas</t>
-  </si>
-  <si>
-    <t>jeffvene@gmail.com</t>
+    <t>ESINTRO</t>
+  </si>
+  <si>
+    <t>CRO150</t>
+  </si>
+  <si>
+    <t>David Solano</t>
+  </si>
+  <si>
+    <t>david@gmail.com</t>
+  </si>
+  <si>
+    <t>CRO156</t>
+  </si>
+  <si>
+    <t>CRO169</t>
+  </si>
+  <si>
+    <t>Stephen Curry Curry</t>
+  </si>
+  <si>
+    <t>BRITISH</t>
+  </si>
+  <si>
+    <t>Daniel Munoz</t>
+  </si>
+  <si>
+    <t>daniel@gmail.com</t>
+  </si>
+  <si>
+    <t>SWEDISH</t>
+  </si>
+  <si>
+    <t>Zlatan Ibrahimovic</t>
+  </si>
+  <si>
+    <t>Gerard Pique</t>
+  </si>
+  <si>
+    <t>pique@barcelona.com</t>
+  </si>
+  <si>
+    <t>GERMANS</t>
+  </si>
+  <si>
+    <t>Jerome Boateng</t>
+  </si>
+  <si>
+    <t>Rebeca Fallas</t>
+  </si>
+  <si>
+    <t>ange@gmail.com</t>
+  </si>
+  <si>
+    <t>Michael Ballack</t>
+  </si>
+  <si>
+    <t>CRO176</t>
+  </si>
+  <si>
+    <t>Roberto Carlos</t>
+  </si>
+  <si>
+    <t>rc23@gmail.com</t>
+  </si>
+  <si>
+    <t>Las Cruces</t>
+  </si>
+  <si>
+    <t>CRO289</t>
+  </si>
+  <si>
+    <t>Palo Verde</t>
+  </si>
+  <si>
+    <t>CRO3658</t>
+  </si>
+  <si>
+    <t>Investigador</t>
+  </si>
+  <si>
+    <t>UNITED STATES</t>
+  </si>
+  <si>
+    <t>Joanna Larson</t>
+  </si>
+  <si>
+    <t>jglarson@umich.edu</t>
+  </si>
+  <si>
+    <t>Angelica Fallas</t>
+  </si>
+  <si>
+    <t>Glen Collier</t>
+  </si>
+  <si>
+    <t>glen-collier@utulsa.edu</t>
+  </si>
+  <si>
+    <t>CRO3908</t>
+  </si>
+  <si>
+    <t>CRO3059</t>
+  </si>
+  <si>
+    <t>CRO3064</t>
+  </si>
+  <si>
+    <t>v v</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -126,21 +240,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.48604801722935" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.96484266008649" customWidth="1"/>
     <col min="3" max="3" width="11.2518583025251" customWidth="1"/>
     <col min="4" max="4" width="14.712888445173" customWidth="1" style="1"/>
     <col min="5" max="5" width="14.712888445173" customWidth="1" style="1"/>
     <col min="6" max="6" width="12.513298034668" customWidth="1"/>
-    <col min="7" max="7" width="12.2360469273158" customWidth="1"/>
-    <col min="8" max="8" width="16.5769141060965" customWidth="1"/>
-    <col min="9" max="9" width="18.3611395699637" customWidth="1"/>
+    <col min="7" max="7" width="13.9486585344587" customWidth="1"/>
+    <col min="8" max="8" width="17.9682824271066" customWidth="1"/>
+    <col min="9" max="9" width="21.0262233189174" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -224,6 +338,522 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>38447</v>
+      </c>
+      <c r="E4" s="1">
+        <v>38450</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>38510</v>
+      </c>
+      <c r="E5" s="1">
+        <v>38575</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E6" s="1">
+        <v>38569</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E7" s="1">
+        <v>38569</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E8" s="1">
+        <v>38569</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E9" s="1">
+        <v>38569</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E10" s="1">
+        <v>38569</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E11" s="1">
+        <v>38569</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E12" s="1">
+        <v>38569</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1">
+        <v>38568</v>
+      </c>
+      <c r="E13" s="1">
+        <v>38569</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1">
+        <v>38716</v>
+      </c>
+      <c r="E14" s="1">
+        <v>38717</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="1">
+        <v>38553</v>
+      </c>
+      <c r="E15" s="1">
+        <v>38555</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="1">
+        <v>38692</v>
+      </c>
+      <c r="E16" s="1">
+        <v>38695</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="1">
+        <v>38692</v>
+      </c>
+      <c r="E17" s="1">
+        <v>38695</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1">
+        <v>38692</v>
+      </c>
+      <c r="E18" s="1">
+        <v>38695</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1">
+        <v>38692</v>
+      </c>
+      <c r="E19" s="1">
+        <v>38695</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1">
+        <v>38692</v>
+      </c>
+      <c r="E20" s="1">
+        <v>38695</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1">
+        <v>38692</v>
+      </c>
+      <c r="E21" s="1">
+        <v>38695</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="1">
+        <v>38709</v>
+      </c>
+      <c r="E22" s="1">
+        <v>38712</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="1">
+        <v>38556</v>
+      </c>
+      <c r="E23" s="1">
+        <v>38556</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="1">
+        <v>38685</v>
+      </c>
+      <c r="E24" s="1">
+        <v>38686</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>